<commit_message>
ccdi 8 input excels added to phs003111
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_PHS-Accession-phs002620_Gender-Male_Race-Unkn.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_PHS-Accession-phs002620_Gender-Male_Race-Unkn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\MarchBranch\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D189564D-AEF6-4A01-A75E-B98283A98582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D17A79-B448-4094-8CA4-C121448C0132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>WebExcel</t>
   </si>
@@ -68,948 +68,6 @@
   </si>
   <si>
     <t>TC01_CCDI_PHS-Accession-phs002620_Gender-Male_Race-Unkn_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>Match (st:study)
-where st.phs_accession in ['phs002620']
-with st
-Call {
-with st
-MATCH (file:clinical_measure_file)
-MATCH (p:participant)-[:of_clinical_measure_file]-(file)
-MATCH (st)&lt;-[:of_participant]-(p)
-OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)
-OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
-OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
-UNWIND apoc.text.split(p.race, ';') AS races
-RETURN DISTINCT
-  file.id as id,
-  p.id as pid,
-  file.clinical_measure_file_id AS file_id,
-  file.dcf_indexd_guid AS guid,
-  file.file_name AS file_name,
-  'Clinical data' AS file_category,
-  file.file_type AS file_type,
-  file.file_description AS file_description,
-  file.file_size AS file_size,
-  file.md5sum AS md5sum,
-  st.study_id AS study_id,
-  st.phs_accession as phs_accession,
-  st.study_acronym as study_acronym,
-  st.study_short_title as study_short_title,
-  p.participant_id AS participant_id,
-  null AS sample_id,
-  null as combined_filters,
-  COLLECT(DISTINCT {
-      race: races,
-      sex_at_birth: p.sex_at_birth,
-      ethnicity: ethnicities
-  }) AS participant_filters,
-  COLLECT(DISTINCT {
-      age_at_diagnosis: dg.age_at_diagnosis,
-      diagnosis_anatomic_site: dg.anatomic_site,
-      disease_phase: dg.disease_phase,
-      diagnosis_classification_system: dg.diagnosis_classification_system,
-      diagnosis_verification_status: dg.diagnosis_verification_status,
-      diagnosis_basis: dg.diagnosis_basis,
-      diagnosis_comment: dg.diagnosis_comment,
-      diagnosis_classification: dg.diagnosis_classification
-  }) AS diagnosis_filters,
-  COLLECT(DISTINCT fu.vital_status) as vital_status,
-  COLLECT(DISTINCT {
-      sample_anatomic_site: sm.anatomic_site,
-      participant_age_at_collection: sm.participant_age_at_collection,
-      sample_tumor_status: sm.sample_tumor_status,
-      tumor_classification: sm.tumor_classification
-  }) AS sample_filters,
-  COLLECT(DISTINCT stf.grant_id) as grant_id,
-  COLLECT(DISTINCT stp.institution) as institution,      
-  null AS library_selection,
-  null AS library_source,
-  null AS library_strategy
-UNION ALL
-with st
-MATCH (file:methylation_array_file)
-MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_methylation_array_file]-(file)
-MATCH (st)&lt;-[:of_participant]-(p)
-OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
-OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
-UNWIND apoc.text.split(p.race, ';') AS races
-with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
-RETURN DISTINCT
-  file.id as id,
-  p.id as pid,
-  file.methylation_array_file_id AS file_id,
-  file.dcf_indexd_guid AS guid,
-  file.file_name AS file_name,
-  'Methylation array' AS file_category,
-  file.file_type AS file_type,
-  file.file_description AS file_description,
-  file.file_size AS file_size,
-  file.md5sum AS md5sum,
-  st.study_id AS study_id,
-  st.phs_accession as phs_accession,
-  st.study_acronym as study_acronym,
-  st.study_short_title as study_short_title,
-  p.participant_id AS participant_id,
-  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
-            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
-  null as combined_filters,
-  COLLECT(DISTINCT {
-      race: races,
-      sex_at_birth: p.sex_at_birth,
-      ethnicity: ethnicities
-  }) AS participant_filters,
-  COLLECT(DISTINCT {
-      age_at_diagnosis: dg.age_at_diagnosis,
-      diagnosis_anatomic_site: dg.anatomic_site,
-      disease_phase: dg.disease_phase,
-      diagnosis_classification_system: dg.diagnosis_classification_system,
-      diagnosis_verification_status: dg.diagnosis_verification_status,
-      diagnosis_basis: dg.diagnosis_basis,
-      diagnosis_comment: dg.diagnosis_comment,
-      diagnosis_classification: dg.diagnosis_classification
-  }) AS diagnosis_filters,
-  COLLECT(DISTINCT fu.vital_status) as vital_status,
-  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })
-            ELSE apoc.coll.union(COLLECT(DISTINCT {
-                              sample_anatomic_site: sm1.anatomic_site,
-                              participant_age_at_collection: sm1.participant_age_at_collection,
-                              sample_tumor_status: sm1.sample_tumor_status,
-                              tumor_classification: sm1.tumor_classification
-                          }), COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })) END AS sample_filters,
-  COLLECT(DISTINCT stf.grant_id) as grant_id,
-  COLLECT(DISTINCT stp.institution) as institution,
-  null AS library_selection,
-  null AS library_source,
-  null AS library_strategy
-UNION ALL
-with st
-MATCH (file:pathology_file)
-MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_pathology_file]-(file)
-MATCH (st)&lt;-[:of_participant]-(p)
-OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
-OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
-UNWIND apoc.text.split(p.race, ';') AS races
-with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
-RETURN DISTINCT
-  file.id as id,
-  p.id as pid,
-  file.pathology_file_id AS file_id,
-  file.dcf_indexd_guid AS guid,
-  file.file_name AS file_name,
-  'Pathology imaging' AS file_category,
-  file.file_type AS file_type,
-  file.file_description AS file_description,
-  file.file_size AS file_size,
-  file.md5sum AS md5sum,
-  st.study_id AS study_id,
-  st.phs_accession as phs_accession,
-  st.study_acronym as study_acronym,
-  st.study_short_title as study_short_title,
-  p.participant_id AS participant_id,
-  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
-            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
-  null as combined_filters,
-  COLLECT(DISTINCT {
-      race: races,
-      sex_at_birth: p.sex_at_birth,
-      ethnicity: ethnicities
-  }) AS participant_filters,
-  COLLECT(DISTINCT {
-      age_at_diagnosis: dg.age_at_diagnosis,
-      diagnosis_anatomic_site: dg.anatomic_site,
-      disease_phase: dg.disease_phase,
-      diagnosis_classification_system: dg.diagnosis_classification_system,
-      diagnosis_verification_status: dg.diagnosis_verification_status,
-      diagnosis_basis: dg.diagnosis_basis,
-      diagnosis_comment: dg.diagnosis_comment,
-      diagnosis_classification: dg.diagnosis_classification
-  }) AS diagnosis_filters,
-  COLLECT(DISTINCT fu.vital_status) as vital_status,
-  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })
-            ELSE apoc.coll.union(COLLECT(DISTINCT {
-                              sample_anatomic_site: sm1.anatomic_site,
-                              participant_age_at_collection: sm1.participant_age_at_collection,
-                              sample_tumor_status: sm1.sample_tumor_status,
-                              tumor_classification: sm1.tumor_classification
-                          }), COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })) END AS sample_filters,
-  COLLECT(DISTINCT stf.grant_id) as grant_id,
-  COLLECT(DISTINCT stp.institution) as institution,
-  file.library_selection AS library_selection,
-  file.library_source AS library_source,
-  file.library_strategy AS library_strategy
-UNION ALL
-with st
-MATCH (file:radiology_file)
-MATCH (p:participant)&lt;-[:of_radiology_file]-(file)
-MATCH (st)&lt;-[:of_participant]-(p)
-OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)
-OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
-OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
-UNWIND apoc.text.split(p.race, ';') AS races
-RETURN DISTINCT
-  file.id as id,
-  p.id as pid,
-  file.radiology_file_id AS file_id,
-  file.dcf_indexd_guid AS guid,
-  file.file_name AS file_name,
-  'Radiology imaging' AS file_category,
-  file.file_type AS file_type,
-  file.file_description AS file_description,
-  file.file_size AS file_size,
-  file.md5sum AS md5sum,
-  st.study_id AS study_id,
-  st.phs_accession as phs_accession,
-  st.study_acronym as study_acronym,
-  st.study_short_title as study_short_title,
-  p.participant_id AS participant_id,
-  null AS sample_id,
-  null as combined_filters,
-  COLLECT(DISTINCT {
-      race: races,
-      sex_at_birth: p.sex_at_birth,
-      ethnicity: ethnicities
-  }) AS participant_filters,
-  COLLECT(DISTINCT {
-      age_at_diagnosis: dg.age_at_diagnosis,
-      diagnosis_anatomic_site: dg.anatomic_site,
-      disease_phase: dg.disease_phase,
-      diagnosis_classification_system: dg.diagnosis_classification_system,
-      diagnosis_verification_status: dg.diagnosis_verification_status,
-      diagnosis_basis: dg.diagnosis_basis,
-      diagnosis_comment: dg.diagnosis_comment,
-      diagnosis_classification: dg.diagnosis_classification
-  }) AS diagnosis_filters,
-  COLLECT(DISTINCT fu.vital_status) as vital_status,
-  COLLECT(DISTINCT {
-      sample_anatomic_site: sm.anatomic_site,
-      participant_age_at_collection: sm.participant_age_at_collection,
-      sample_tumor_status: sm.sample_tumor_status,
-      tumor_classification: sm.tumor_classification
-  }) AS sample_filters,
-  COLLECT(DISTINCT stf.grant_id) as grant_id,
-  COLLECT(DISTINCT stp.institution) as institution,
-  null AS library_selection,
-  null AS library_source,
-  null AS library_strategy
-UNION ALL
-with st
-MATCH (file:single_cell_sequencing_file)
-MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_single_cell_sequencing_file]-(file)
-MATCH (st)&lt;-[:of_participant]-(p)
-OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
-OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
-UNWIND apoc.text.split(p.race, ';') AS races
-with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
-RETURN DISTINCT
-  file.id as id,
-  p.id as pid,
-  file.single_cell_sequencing_file_id AS file_id,
-  file.dcf_indexd_guid AS guid,
-  file.file_name AS file_name,
-  'Single Cell Sequencing' AS file_category,
-  file.file_type AS file_type,
-  file.file_description AS file_description,
-  file.file_size AS file_size,
-  file.md5sum AS md5sum,
-  st.study_id AS study_id,
-  st.phs_accession as phs_accession,
-  st.study_acronym as study_acronym,
-  st.study_short_title as study_short_title,
-  p.participant_id AS participant_id,
-  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
-            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
-  null as combined_filters,
-  COLLECT(DISTINCT {
-      race: races,
-      sex_at_birth: p.sex_at_birth,
-      ethnicity: ethnicities
-  }) AS participant_filters,
-  COLLECT(DISTINCT {
-      age_at_diagnosis: dg.age_at_diagnosis,
-      diagnosis_anatomic_site: dg.anatomic_site,
-      disease_phase: dg.disease_phase,
-      diagnosis_classification_system: dg.diagnosis_classification_system,
-      diagnosis_verification_status: dg.diagnosis_verification_status,
-      diagnosis_basis: dg.diagnosis_basis,
-      diagnosis_comment: dg.diagnosis_comment,
-      diagnosis_classification: dg.diagnosis_classification
-  }) AS diagnosis_filters,
-  COLLECT(DISTINCT fu.vital_status) as vital_status,
-  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })
-            ELSE apoc.coll.union(COLLECT(DISTINCT {
-                              sample_anatomic_site: sm1.anatomic_site,
-                              participant_age_at_collection: sm1.participant_age_at_collection,
-                              sample_tumor_status: sm1.sample_tumor_status,
-                              tumor_classification: sm1.tumor_classification
-                          }), COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })) END AS sample_filters,
-  COLLECT(DISTINCT stf.grant_id) as grant_id,
-  COLLECT(DISTINCT stp.institution) as institution,
-  file.library_selection AS library_selection,
-  file.library_source AS library_source,
-  file.library_strategy AS library_strategy
-UNION ALL
-with st
-MATCH (file:sequencing_file)
-MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_sequencing_file]-(file)
-MATCH (st)&lt;-[:of_participant]-(p)
-OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
-OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
-UNWIND apoc.text.split(p.race, ';') AS races
-with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
-RETURN DISTINCT
-  file.id as id,
-  p.id as pid,
-  file.sequencing_file_id AS file_id,
-  file.dcf_indexd_guid AS guid,
-  file.file_name AS file_name,
-  'Sequencing' AS file_category,
-  file.file_type AS file_type,
-  file.file_description AS file_description,
-  file.file_size AS file_size,
-  file.md5sum AS md5sum,
-  st.study_id AS study_id,
-  st.phs_accession as phs_accession,
-  st.study_acronym as study_acronym,
-  st.study_short_title as study_short_title,
-  p.participant_id AS participant_id,
-  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
-            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
-  null as combined_filters,
-  COLLECT(DISTINCT {
-      race: races,
-      sex_at_birth: p.sex_at_birth,
-      ethnicity: ethnicities
-  }) AS participant_filters,
-  COLLECT(DISTINCT {
-      age_at_diagnosis: dg.age_at_diagnosis,
-      diagnosis_anatomic_site: dg.anatomic_site,
-      disease_phase: dg.disease_phase,
-      diagnosis_classification_system: dg.diagnosis_classification_system,
-      diagnosis_verification_status: dg.diagnosis_verification_status,
-      diagnosis_basis: dg.diagnosis_basis,
-      diagnosis_comment: dg.diagnosis_comment,
-      diagnosis_classification: dg.diagnosis_classification
-  }) AS diagnosis_filters,
-  COLLECT(DISTINCT fu.vital_status) as vital_status,
-  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })
-            ELSE apoc.coll.union(COLLECT(DISTINCT {
-                              sample_anatomic_site: sm1.anatomic_site,
-                              participant_age_at_collection: sm1.participant_age_at_collection,
-                              sample_tumor_status: sm1.sample_tumor_status,
-                              tumor_classification: sm1.tumor_classification
-                          }), COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })) END AS sample_filters,
-  COLLECT(DISTINCT stf.grant_id) as grant_id,
-  COLLECT(DISTINCT stp.institution) as institution,
-  file.library_selection AS library_selection,
-  file.library_source AS library_source,
-  file.library_strategy AS library_strategy
-UNION ALL
-with st
-MATCH (file:cytogenomic_file)
-MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_cytogenomic_file]-(file)
-MATCH (st)&lt;-[:of_participant]-(p)
-OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
-OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
-UNWIND apoc.text.split(p.race, ';') AS races
-with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
-RETURN DISTINCT
-  file.id as id,
-  p.id as pid,
-  file.cytogenomic_file_id AS file_id,
-  file.dcf_indexd_guid AS guid,
-  file.file_name AS file_name,
-  'Cytogenomic' AS file_category,
-  file.file_type AS file_type,
-  file.file_description AS file_description,
-  file.file_size AS file_size,
-  file.md5sum AS md5sum,
-  st.study_id AS study_id,
-  st.phs_accession as phs_accession,
-  st.study_acronym as study_acronym,
-  st.study_short_title as study_short_title,
-  p.participant_id AS participant_id,
-  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
-            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
-  null as combined_filters,
-  COLLECT(DISTINCT {
-      race: races,
-      sex_at_birth: p.sex_at_birth,
-      ethnicity: ethnicities
-  }) AS participant_filters,
-  COLLECT(DISTINCT {
-      age_at_diagnosis: dg.age_at_diagnosis,
-      diagnosis_anatomic_site: dg.anatomic_site,
-      disease_phase: dg.disease_phase,
-      diagnosis_classification_system: dg.diagnosis_classification_system,
-      diagnosis_verification_status: dg.diagnosis_verification_status,
-      diagnosis_basis: dg.diagnosis_basis,
-      diagnosis_comment: dg.diagnosis_comment,
-      diagnosis_classification: dg.diagnosis_classification
-  }) AS diagnosis_filters,
-  COLLECT(DISTINCT fu.vital_status) as vital_status,
-  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })
-            ELSE apoc.coll.union(COLLECT(DISTINCT {
-                              sample_anatomic_site: sm1.anatomic_site,
-                              participant_age_at_collection: sm1.participant_age_at_collection,
-                              sample_tumor_status: sm1.sample_tumor_status,
-                              tumor_classification: sm1.tumor_classification
-                          }), COLLECT(DISTINCT {
-                              sample_anatomic_site: sm.anatomic_site,
-                              participant_age_at_collection: sm.participant_age_at_collection,
-                              sample_tumor_status: sm.sample_tumor_status,
-                              tumor_classification: sm.tumor_classification
-                          })) END AS sample_filters,
-  COLLECT(DISTINCT stf.grant_id) as grant_id,
-  COLLECT(DISTINCT stp.institution) as institution,
-  null AS library_selection,
-  null AS library_source,
-  null AS library_strategy
-UNION ALL
-with st
-MATCH (file)
-WHERE (file:sequencing_file OR file:pathology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
-MATCH (st)&lt;-[:of_cell_line|of_pdx]-(cl)&lt;--(sm:sample)
-Where (cl: cell_line or cl: pdx)
-MATCH (sm)&lt;--(file)
-OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-OPTIONAL MATCH (st)&lt;--(p:participant)&lt;-[:of_diagnosis]-(dg:diagnosis)
-OPTIONAL MATCH (st)&lt;--(p)&lt;-[:of_follow_up]-(fu:follow_up)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-with file, sm, st, fu, dg, stf, stp
-RETURN DISTINCT
-  file.id as id,
-  null as pid,
-  CASE LABELS(file)[0]
-        WHEN 'sequencing_file' THEN file.sequencing_file_id
-        WHEN 'single_cell_sequencing_file' THEN file.single_cell_sequencing_file_id
-        WHEN 'cytogenomic_file' THEN file.cytogenomic_file_id
-        WHEN 'pathology_file' THEN file.pathology_file_id
-        WHEN 'methylation_array_file' THEN file.methylation_array_file_id END AS file_id,
-  file.dcf_indexd_guid AS guid,
-  file.file_name AS file_name,
-  CASE LABELS(file)[0]
-        WHEN 'sequencing_file' THEN 'Sequencing'
-        WHEN 'single_cell_sequencing_file' THEN 'Single Cell Sequencing'
-        WHEN 'cytogenomic_file' THEN 'Cytogenomic'
-        WHEN 'pathology_file' THEN 'Pathology imaging'
-        WHEN 'methylation_array_file' THEN 'Methylation array' END AS file_category,
-  file.file_type AS file_type,
-  file.file_description AS file_description,
-  file.file_size AS file_size,
-  file.md5sum AS md5sum,
-  st.study_id AS study_id,
-  st.phs_accession as phs_accession,
-  st.study_acronym as study_acronym,
-  st.study_short_title as study_short_title,
-  null AS participant_id,
-  sm.sample_id AS sample_id,
-  null as combined_filters,
-  null AS participant_filters,
-  COLLECT(DISTINCT {
-      age_at_diagnosis: dg.age_at_diagnosis,
-      diagnosis_anatomic_site: dg.anatomic_site,
-      disease_phase: dg.disease_phase,
-      diagnosis_classification_system: dg.diagnosis_classification_system,
-      diagnosis_verification_status: dg.diagnosis_verification_status,
-      diagnosis_basis: dg.diagnosis_basis,
-      diagnosis_comment: dg.diagnosis_comment,
-      diagnosis_classification: dg.diagnosis_classification
-  }) AS diagnosis_filters,
-  COLLECT(DISTINCT fu.vital_status) as vital_status,
-  COLLECT(DISTINCT {
-      sample_anatomic_site: sm.anatomic_site,
-      participant_age_at_collection: sm.participant_age_at_collection,
-      sample_tumor_status: sm.sample_tumor_status,
-      tumor_classification: sm.tumor_classification
-  }) AS sample_filters,
-  COLLECT(DISTINCT stf.grant_id) as grant_id,
-  COLLECT(DISTINCT stp.institution) as institution,
-  CASE LABELS(file)[0]
-            WHEN 'sequencing_file' THEN file.library_selection
-            WHEN 'single_cell_sequencing_file' THEN file.library_selection
-            ELSE null END AS library_selection,
-  CASE LABELS(file)[0]
-            WHEN 'sequencing_file' THEN file.library_source
-            WHEN 'single_cell_sequencing_file' THEN file.library_source
-            ELSE null END AS library_source,
-  CASE LABELS(file)[0]
-            WHEN 'sequencing_file' THEN file.library_strategy
-            WHEN 'single_cell_sequencing_file' THEN file.library_strategy
-            ELSE null END AS library_strategy
-}
-with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, pid, participant_id, sample_id, participant_filters,diagnosis_filters, vital_status, sample_filters, grant_id, institution,library_selection,library_source,library_strategy
-unwind participant_filters as participant_filter
-with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, pid, participant_id, sample_id, participant_filter,diagnosis_filters, vital_status, sample_filters, grant_id, institution,library_selection,library_source,library_strategy
-where participant_filter.sex_at_birth in ['Male'] and ANY(element IN ['Unknown'] WHERE element IN participant_filter.race) 
-unwind diagnosis_filters as diagnosis_filter
-with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, pid, participant_id, sample_id,diagnosis_filter, vital_status, sample_filters, grant_id, institution,library_selection,library_source,library_strategy
- with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, pid, participant_id, sample_id, vital_status, sample_filters, grant_id, institution,library_selection,library_source,library_strategy
-unwind sample_filters as sample_filter
-with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, pid, participant_id, sample_id, sample_filter, grant_id, institution,library_selection,library_source,library_strategy
-with distinct id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, pid, participant_id, sample_id, grant_id, institution,library_selection,library_source,library_strategy
-call {
-  with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, pid, participant_id, sample_id, grant_id, institution,library_selection,library_source,library_strategy
-  return id as fid, guid as dig, file_name as fn, file_category as fc, file_type as ft, file_description as fd, file_size as fsize, md5sum as md5, study_id as sid, phs_accession as pa, study_acronym as sa, study_short_title as sst, pid as u_p_id, participant_id as p_id, sample_id as smid, grant_id as gid, institution as istt,library_selection as ls,library_source as lis,library_strategy as listr
-  UNION ALL
-  with study_id
-  MATCH (file:clinical_measure_file)
-  MATCH (stu:study)&lt;-[:of_clinical_measure_file]-(file)
-  where stu.study_id = study_id
-  OPTIONAL MATCH (stu)&lt;-[:of_study_personnel]-(stp:study_personnel)
-  OPTIONAL MATCH (stu)&lt;-[:of_study_funding]-(stf:study_funding)
-  With file, stu, stf, stp
-  RETURN DISTINCT
-    file.id as fid,
-    file.dcf_indexd_guid AS dig,
-    file.file_name AS fn,
-    'Clinical data' AS fc,
-    file.file_type AS ft,
-    file.file_description AS fd,
-    file.file_size AS fsize,
-    file.md5sum AS md5,
-    stu.study_id AS sid,
-    stu.phs_accession as pa,
-    stu.study_acronym as sa,
-    stu.study_short_title as sst,
-    null AS p_id,
-    null AS u_p_id,
-    null AS smid,
-    COLLECT(DISTINCT stf.grant_id) as gid,
-    COLLECT(DISTINCT stp.institution) as istt,
-    null AS ls,
-    null AS lis,
-    null AS listr
-}
-with fid as id, dig as guid, fn as file_name, fc as file_category, ft as file_type, fd as file_description, fsize as file_size, md5 as md5sum, sid as study_id, pa as phs_accession, sa as study_acronym, sst as study_short_title, u_p_id as unique_participant_id, p_id as participant_id, smid as sample_id, gid as grant_id, istt as institution,ls as library_selection,lis as library_source,listr as library_strategy
- with DISTINCT id, study_id, unique_participant_id, sample_id
-with id, study_id, unique_participant_id, case sample_id when null then [null] else apoc.text.split(sample_id, ',') end as sample_ids
-unwind sample_ids as single_sample_id
-return  count(distinct study_id) as Studies, count(distinct unique_participant_id) as Participants, count(distinct single_sample_id) as Samples, count(distinct id) as Files</t>
-  </si>
-  <si>
-    <t>MATCH (p:participant)--&gt;(st:study)
-where st.phs_accession in ['phs002620']
-optional MATCH (p)&lt;-[:of_sample]-(sm1:sample)&lt;--(cl)&lt;--(sm2:sample)
-WHERE (cl: cell_line or cl: pdx)
-optional Match (sm2)&lt;--(file)
-WHERE (file: sequencing_file OR file:pathology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file) 
-with p, case COLLECT(distinct sm1) when [] then []
-                else COLLECT(DISTINCT {
-                        sample_anatomic_site: sm1.anatomic_site,
-                        participant_age_at_collection: sm1.participant_age_at_collection,
-                        sample_tumor_status: sm1.sample_tumor_status,
-                        tumor_classification: sm1.tumor_classification,
-                        assay_method: CASE LABELS(file)[0]
-                                  WHEN 'sequencing_file' THEN 'Sequencing'
-                                  WHEN 'single_cell_sequencing_file' THEN 'Single Cell Sequencing'
-                                  WHEN 'cytogenomic_file' THEN 'Cytogenomic'
-                                  WHEN 'pathology_file' THEN 'Pathology imaging'
-                                  WHEN 'methylation_array_file' THEN 'Methylation array'
-                                  ELSE null END,
-                        file_type: CASE LABELS(file)[0]
-                                  When null then null
-                                  else file.file_type end,
-                        library_selection: CASE LABELS(file)[0]
-                                      WHEN 'sequencing_file' THEN file.library_selection
-                                      WHEN 'single_cell_sequencing_file' THEN file.library_selection
-                                      ELSE null END,
-                        library_source: CASE LABELS(file)[0]
-                                      WHEN 'sequencing_file' THEN file.library_source
-                                      WHEN 'single_cell_sequencing_file' THEN file.library_source
-                                      ELSE null END,
-                        library_strategy: CASE LABELS(file)[0]
-                                      WHEN 'sequencing_file' THEN file.library_strategy
-                                      WHEN 'single_cell_sequencing_file' THEN file.library_strategy
-                                      ELSE null END
-                    }) end AS sample1,
-                    case COLLECT(distinct sm2) 
-                    when [] then []
-                    else COLLECT(DISTINCT {
-                        sample_anatomic_site: sm2.anatomic_site,
-                        participant_age_at_collection: sm2.participant_age_at_collection,
-                        sample_tumor_status: sm2.sample_tumor_status,
-                        tumor_classification: sm2.tumor_classification,
-                        assay_method: CASE LABELS(file)[0]
-                                  WHEN 'sequencing_file' THEN 'Sequencing'
-                                  WHEN 'single_cell_sequencing_file' THEN 'Single Cell Sequencing'
-                                  WHEN 'cytogenomic_file' THEN 'Cytogenomic'
-                                  WHEN 'pathology_file' THEN 'Pathology imaging'
-                                  WHEN 'methylation_array_file' THEN 'Methylation array'
-                                  ELSE null END,
-                        file_type: CASE LABELS(file)[0]
-                                  When null then null
-                                  else file.file_type end,
-                        library_selection: CASE LABELS(file)[0]
-                                      WHEN 'sequencing_file' THEN file.library_selection
-                                      WHEN 'single_cell_sequencing_file' THEN file.library_selection
-                                      ELSE null END,
-                        library_source: CASE LABELS(file)[0]
-                                      WHEN 'sequencing_file' THEN file.library_source
-                                      WHEN 'single_cell_sequencing_file' THEN file.library_source
-                                      ELSE null END,
-                        library_strategy: CASE LABELS(file)[0]
-                                      WHEN 'sequencing_file' THEN file.library_strategy
-                                      WHEN 'single_cell_sequencing_file' THEN file.library_strategy
-                                      ELSE null END
-                    }) end AS sample2
-with p, apoc.coll.union(sample1,sample2) as cell_line_pdx_file_filters
-OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)&lt;--(file)
-WHERE (file: sequencing_file OR file:pathology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
-with p, cell_line_pdx_file_filters, COLLECT(DISTINCT {
-              sample_anatomic_site: sm.anatomic_site,
-              participant_age_at_collection: sm.participant_age_at_collection,
-              sample_tumor_status: sm.sample_tumor_status,
-              tumor_classification: sm.tumor_classification,
-              assay_method: CASE LABELS(file)[0]
-                        WHEN 'sequencing_file' THEN 'Sequencing'
-                        WHEN 'single_cell_sequencing_file' THEN 'Single Cell Sequencing'
-                        WHEN 'cytogenomic_file' THEN 'Cytogenomic'
-                        WHEN 'pathology_file' THEN 'Pathology imaging'
-                        WHEN 'methylation_array_file' THEN 'Methylation array' END,
-              file_type: file.file_type,
-              library_selection: CASE LABELS(file)[0]
-                            WHEN 'sequencing_file' THEN file.library_selection
-                            WHEN 'single_cell_sequencing_file' THEN file.library_selection
-                            ELSE null END,
-              library_source: CASE LABELS(file)[0]
-                            WHEN 'sequencing_file' THEN file.library_source
-                              WHEN 'single_cell_sequencing_file' THEN file.library_source
-                            ELSE null END,
-              library_strategy: CASE LABELS(file)[0]
-                            WHEN 'sequencing_file' THEN file.library_strategy
-                            WHEN 'single_cell_sequencing_file' THEN file.library_strategy
-                            ELSE null END
-          }) AS general_file_filters
-OPTIONAL Match (p)&lt;-[:of_sample]-(sm:sample)
-OPTIONAL MATCH (p)&lt;-[:of_clinical_measure_file]-(file1:clinical_measure_file)
-with p, cell_line_pdx_file_filters, general_file_filters,sm, COLLECT(DISTINCT file1.file_type) as file1_types
-UNWIND (case file1_types when [] then [null] else file1_types end)  AS types_1
-with p, cell_line_pdx_file_filters, general_file_filters, COLLECT(DISTINCT {
-          sample_anatomic_site: sm.anatomic_site,
-          participant_age_at_collection: sm.participant_age_at_collection,
-          sample_tumor_status: sm.sample_tumor_status,
-          tumor_classification: sm.tumor_classification,
-          assay_method: CASE types_1 when null then null else 'Clinical data' end,
-          file_type: types_1,
-          library_selection: null,
-          library_source: null,
-          library_strategy: null
-  }) as participant_clinical_measure_file_filters
-OPTIONAL Match (p)&lt;-[:of_sample]-(sm:sample)
-OPTIONAL MATCH (p)&lt;-[:of_radiology_file]-(file1:radiology_file)
-with p, cell_line_pdx_file_filters, general_file_filters, participant_clinical_measure_file_filters, sm, COLLECT(DISTINCT file1.file_type) as file1_types
-UNWIND (case file1_types when [] then [null] else file1_types end)  AS types_1
-with p, cell_line_pdx_file_filters, general_file_filters, participant_clinical_measure_file_filters, COLLECT(DISTINCT {
-          sample_anatomic_site: sm.anatomic_site,
-          participant_age_at_collection: sm.participant_age_at_collection,
-          sample_tumor_status: sm.sample_tumor_status,
-          tumor_classification: sm.tumor_classification,
-          assay_method: CASE types_1 when null then null else 'Radiology imaging' end,
-          file_type: types_1,
-          library_selection: null,
-          library_source: null,
-          library_strategy: null
-  }) as participant_radiology_file_filters
-OPTIONAL MATCH (p)&lt;-[*..4]-(file)
-WHERE (file:clinical_measure_file OR file: sequencing_file OR file:pathology_file OR file:radiology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
-OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
-OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
-OPTIONAL MATCH (st:study)&lt;-[:of_participant]-(p)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-WITH p, cell_line_pdx_file_filters, general_file_filters, participant_clinical_measure_file_filters, participant_radiology_file_filters, file, fu, st, stf, stp, dg
-with DISTINCT
-  p.id as id,
-  p.participant_id as participant_id,
-  apoc.text.split(p.race, ';') as race,
-  p.race as race_str,
-  p.sex_at_birth as sex_at_birth,
-  p.ethnicity as ethnicity_str,
-  apoc.text.split(p.ethnicity, ';') as ethnicity,
-  p.alternate_participant_id as alternate_participant_id,
-  COLLECT(DISTINCT {
-      age_at_diagnosis: dg.age_at_diagnosis,
-      diagnosis_anatomic_site: dg.anatomic_site,
-      disease_phase: dg.disease_phase,
-      diagnosis_classification_system: dg.diagnosis_classification_system,
-      diagnosis_verification_status: dg.diagnosis_verification_status,
-      diagnosis_basis: dg.diagnosis_basis,
-      diagnosis_comment: dg.diagnosis_comment,
-      diagnosis_classification: dg.diagnosis_classification
-  }) AS diagnosis_filters,
-  COLLECT(DISTINCT fu.vital_status) as vital_status,
-  apoc.coll.union(cell_line_pdx_file_filters, general_file_filters) + participant_clinical_measure_file_filters + participant_radiology_file_filters AS sample_file_filters,
-  st.study_id as study_id,
-  st.phs_accession as phs_accession,
-  COLLECT(DISTINCT stf.grant_id) as grant_id,
-  COLLECT(DISTINCT stp.institution) as institution,
-  st.study_acronym as study_acronym,
-  st.study_short_title as study_short_title
-  with id, participant_id, phs_accession, sex_at_birth, race_str, ethnicity_str, race, ethnicity, alternate_participant_id, diagnosis_filters, vital_status, sample_file_filters
-  where   sex_at_birth in ['Male'] and ANY(element IN ['Unknown'] WHERE element IN race) 
-    with distinct id, participant_id, phs_accession, sex_at_birth, race_str, ethnicity_str, alternate_participant_id
-  return
-  coalesce(participant_id, '') AS `Participant ID`,
-  coalesce(phs_accession, '') AS `Study ID`,
-  coalesce(sex_at_birth, '') AS `Sex` ,
-  coalesce(race_str, '') AS `Race`,
-  coalesce(ethnicity_str, '') AS `Ethnicity` ,
-  coalesce(alternate_participant_id, '') AS `Alternate ID`
-  Order by participant_id Limit 100</t>
-  </si>
-  <si>
-    <t>MATCH (p:participant)--&gt;(st:study)
-where st.phs_accession in ['phs002620']
-optional MATCH (p)&lt;-[:of_sample]-(sm1:sample)&lt;--(cl)&lt;--(sm2:sample)
-WHERE (cl: cell_line or cl: pdx)
-optional Match (sm2)&lt;--(file)
-WHERE (file: sequencing_file OR file:pathology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file) 
-with p, case COLLECT(distinct sm1) when [] then []
-              else COLLECT(DISTINCT {
-                      sample_anatomic_site: sm1.anatomic_site,
-                      participant_age_at_collection: sm1.participant_age_at_collection,
-                      sample_tumor_status: sm1.sample_tumor_status,
-                      tumor_classification: sm1.tumor_classification,
-                      assay_method: CASE LABELS(file)[0]
-                                WHEN 'sequencing_file' THEN 'Sequencing'
-                                WHEN 'single_cell_sequencing_file' THEN 'Single Cell Sequencing'
-                                WHEN 'cytogenomic_file' THEN 'Cytogenomic'
-                                WHEN 'pathology_file' THEN 'Pathology imaging'
-                                WHEN 'methylation_array_file' THEN 'Methylation array'
-                                ELSE null END,
-                      file_type: CASE LABELS(file)[0]
-                                When null then null
-                                else file.file_type end,
-                      library_selection: CASE LABELS(file)[0]
-                                    WHEN 'sequencing_file' THEN file.library_selection
-                                    WHEN 'single_cell_sequencing_file' THEN file.library_selection
-                                    ELSE null END,
-                      library_source: CASE LABELS(file)[0]
-                                    WHEN 'sequencing_file' THEN file.library_source
-                                    WHEN 'single_cell_sequencing_file' THEN file.library_source
-                                    ELSE null END,
-                      library_strategy: CASE LABELS(file)[0]
-                                    WHEN 'sequencing_file' THEN file.library_strategy
-                                    WHEN 'single_cell_sequencing_file' THEN file.library_strategy
-                                    ELSE null END
-                  }) end AS sample1,
-                  case COLLECT(distinct sm2) 
-                  when [] then []
-                  else COLLECT(DISTINCT {
-                      sample_anatomic_site: sm2.anatomic_site,
-                      participant_age_at_collection: sm2.participant_age_at_collection,
-                      sample_tumor_status: sm2.sample_tumor_status,
-                      tumor_classification: sm2.tumor_classification,
-                      assay_method: CASE LABELS(file)[0]
-                                WHEN 'sequencing_file' THEN 'Sequencing'
-                                WHEN 'single_cell_sequencing_file' THEN 'Single Cell Sequencing'
-                                WHEN 'cytogenomic_file' THEN 'Cytogenomic'
-                                WHEN 'pathology_file' THEN 'Pathology imaging'
-                                WHEN 'methylation_array_file' THEN 'Methylation array'
-                                ELSE null END,
-                      file_type: CASE LABELS(file)[0]
-                                When null then null
-                                else file.file_type end,
-                      library_selection: CASE LABELS(file)[0]
-                                    WHEN 'sequencing_file' THEN file.library_selection
-                                    WHEN 'single_cell_sequencing_file' THEN file.library_selection
-                                    ELSE null END,
-                      library_source: CASE LABELS(file)[0]
-                                    WHEN 'sequencing_file' THEN file.library_source
-                                    WHEN 'single_cell_sequencing_file' THEN file.library_source
-                                    ELSE null END,
-                      library_strategy: CASE LABELS(file)[0]
-                                    WHEN 'sequencing_file' THEN file.library_strategy
-                                    WHEN 'single_cell_sequencing_file' THEN file.library_strategy
-                                    ELSE null END
-                  }) end AS sample2
-with p, apoc.coll.union(sample1,sample2) as cell_line_pdx_file_filters
-OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)&lt;--(file)
-WHERE (file: sequencing_file OR file:pathology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
-with p, cell_line_pdx_file_filters, COLLECT(DISTINCT {
-              sample_anatomic_site: sm.anatomic_site,
-              participant_age_at_collection: sm.participant_age_at_collection,
-              sample_tumor_status: sm.sample_tumor_status,
-              tumor_classification: sm.tumor_classification,
-              assay_method: CASE LABELS(file)[0]
-                        WHEN 'sequencing_file' THEN 'Sequencing'
-                        WHEN 'single_cell_sequencing_file' THEN 'Single Cell Sequencing'
-                        WHEN 'cytogenomic_file' THEN 'Cytogenomic'
-                        WHEN 'pathology_file' THEN 'Pathology imaging'
-                        WHEN 'methylation_array_file' THEN 'Methylation array' END,
-              file_type: file.file_type,
-              library_selection: CASE LABELS(file)[0]
-                            WHEN 'sequencing_file' THEN file.library_selection
-                            WHEN 'single_cell_sequencing_file' THEN file.library_selection
-                            ELSE null END,
-              library_source: CASE LABELS(file)[0]
-                            WHEN 'sequencing_file' THEN file.library_source
-                            WHEN 'single_cell_sequencing_file' THEN file.library_source
-                            ELSE null END,
-              library_strategy: CASE LABELS(file)[0]
-                            WHEN 'sequencing_file' THEN file.library_strategy
-                            WHEN 'single_cell_sequencing_file' THEN file.library_strategy
-                            ELSE null END
-          }) AS general_file_filters
-OPTIONAL Match (p)&lt;-[:of_sample]-(sm:sample)
-OPTIONAL MATCH (p)&lt;-[:of_clinical_measure_file]-(file1:clinical_measure_file)
-with p, cell_line_pdx_file_filters, general_file_filters,sm, COLLECT(DISTINCT file1.file_type) as file1_types
-UNWIND (case file1_types when [] then [null] else file1_types end)  AS types_1
-with p, cell_line_pdx_file_filters, general_file_filters, COLLECT(DISTINCT {
-          sample_anatomic_site: sm.anatomic_site,
-          participant_age_at_collection: sm.participant_age_at_collection,
-          sample_tumor_status: sm.sample_tumor_status,
-          tumor_classification: sm.tumor_classification,
-          assay_method: CASE types_1 when null then null else 'Clinical data' end,
-          file_type: types_1,
-          library_selection: null,
-          library_source: null,
-          library_strategy: null
-  }) as participant_clinical_measure_file_filters
-OPTIONAL Match (p)&lt;-[:of_sample]-(sm:sample)
-OPTIONAL MATCH (p)&lt;-[:of_radiology_file]-(file1:radiology_file)
-with p, cell_line_pdx_file_filters, general_file_filters, participant_clinical_measure_file_filters, sm, COLLECT(DISTINCT file1.file_type) as file1_types
-UNWIND (case file1_types when [] then [null] else file1_types end)  AS types_1
-with p, cell_line_pdx_file_filters, general_file_filters, participant_clinical_measure_file_filters, COLLECT(DISTINCT {
-          sample_anatomic_site: sm.anatomic_site,
-          participant_age_at_collection: sm.participant_age_at_collection,
-          sample_tumor_status: sm.sample_tumor_status,
-          tumor_classification: sm.tumor_classification,
-          assay_method: CASE types_1 when null then null else 'Radiology imaging' end,
-          file_type: types_1,
-          library_selection: null,
-          library_source: null,
-          library_strategy: null
-  }) as participant_radiology_file_filters
-MATCH (dg:diagnosis)
-MATCH (p)&lt;-[:of_diagnosis]-(dg)
-OPTIONAL MATCH (p)&lt;-[*..4]-(file)
-WHERE (file:clinical_measure_file OR file: sequencing_file OR file:pathology_file OR file:radiology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
-OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
-with p, cell_line_pdx_file_filters, general_file_filters, participant_clinical_measure_file_filters,participant_radiology_file_filters, dg, file, fu order by fu.age_at_follow_up desc
-OPTIONAL MATCH (st:study)&lt;-[:of_participant]-(p)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-WITH p, cell_line_pdx_file_filters, general_file_filters, participant_clinical_measure_file_filters,participant_radiology_file_filters, file, fu, st, stf, stp, dg
-with DISTINCT
-  dg.id as id,
-  dg.diagnosis_classification as diagnosis_classification,
-  dg.disease_phase as disease_phase,
-  dg.diagnosis_classification_system as diagnosis_classification_system,
-  dg.diagnosis_verification_status as diagnosis_verification_status,
-  dg.diagnosis_basis as diagnosis_basis,
-  dg.diagnosis_comment as diagnosis_comment,
-  dg.anatomic_site as diagnosis_anatomic_site,
-  dg.age_at_diagnosis as age_at_diagnosis,
-  p.participant_id as participant_id,
-  apoc.text.split(p.race, ';') as race,
-  p.sex_at_birth as sex_at_birth,
-  apoc.text.split(p.ethnicity, ';') as ethnicity,
-  st.study_id as study_id,
-  st.phs_accession as phs_accession,
-  st.study_acronym as study_acronym,
-  st.study_short_title as study_short_title,
-  head(collect(distinct fu.vital_status)) as last_vital_status,
-  COLLECT(DISTINCT fu.vital_status) as vital_status,
-  apoc.coll.union(cell_line_pdx_file_filters, general_file_filters) + participant_clinical_measure_file_filters + participant_radiology_file_filters AS sample_file_filters,
-  COLLECT(DISTINCT stf.grant_id) as grant_id,
-  COLLECT(DISTINCT stp.institution) as institution
-with id, participant_id, phs_accession, sex_at_birth, race, ethnicity, diagnosis_classification, diagnosis_classification_system, diagnosis_verification_status, diagnosis_basis, diagnosis_comment, disease_phase, diagnosis_anatomic_site, age_at_diagnosis, last_vital_status, vital_status, sample_file_filters
-where   sex_at_birth in ['Male'] and ANY(element IN ['Unknown'] WHERE element IN race)  
-with id, participant_id, phs_accession, diagnosis_classification, diagnosis_classification_system, diagnosis_verification_status, diagnosis_basis, diagnosis_comment, disease_phase, diagnosis_anatomic_site, age_at_diagnosis, last_vital_status, vital_status, sample_file_filters
-with id, participant_id, phs_accession, diagnosis_classification, diagnosis_classification_system, diagnosis_verification_status, diagnosis_basis, diagnosis_comment, disease_phase, diagnosis_anatomic_site, age_at_diagnosis, last_vital_status, vital_status, sample_file_filters
-unwind sample_file_filters as sample_file_filter
-with id, participant_id, phs_accession, diagnosis_classification, diagnosis_classification_system, diagnosis_verification_status, diagnosis_basis, diagnosis_comment, disease_phase, diagnosis_anatomic_site, age_at_diagnosis, last_vital_status, sample_file_filter
- with distinct id, participant_id, phs_accession, diagnosis_classification, diagnosis_classification_system, diagnosis_verification_status, diagnosis_basis, diagnosis_comment, disease_phase, diagnosis_anatomic_site, age_at_diagnosis, last_vital_status
-return
-coalesce(participant_id, '') as `Participant ID`,
-coalesce(phs_accession, '') as `Study ID`,
-coalesce(diagnosis_classification, '') as `Diagnosis`,
-coalesce(diagnosis_classification_system, '') as `Diagnosis Classification System`,
-coalesce(diagnosis_verification_status, '') as `Diagnosis Verification Status`,
-coalesce(diagnosis_basis, '') as `Diagnosis Basis`,
-coalesce(diagnosis_comment, '') as `Diagnosis Comment`,
-coalesce(disease_phase, '') as `Disease Phase`,
-coalesce(diagnosis_anatomic_site, '') as `Anatomic Site`,
-case age_at_diagnosis when -999 then 'Not Reported' else coalesce(age_at_diagnosis, '') end as `Age at diagnosis (days)`,
-coalesce(last_vital_status, '') as `Vital Status`
-Order by participant_id limit 100</t>
   </si>
   <si>
     <t>MATCH (p:participant)--&gt;(st:study)
@@ -2020,6 +1078,775 @@
 guid As `GUID`,
 md5sum As `MD5Sum`
 ORDER BY file_name limit 100</t>
+  </si>
+  <si>
+    <t>Match (st:study)
+where st.phs_accession in ['phs002620']
+with st
+Call {
+with st
+MATCH (file:clinical_measure_file)
+MATCH (p:participant)-[:of_clinical_measure_file]-(file)
+MATCH (st)&lt;-[:of_participant]-(p)
+OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)
+OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
+OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
+UNWIND apoc.text.split(p.race, ';') AS races
+RETURN DISTINCT
+  file.id as id,
+  p.id as pid,
+  file.clinical_measure_file_id AS file_id,
+  file.dcf_indexd_guid AS guid,
+  file.file_name AS file_name,
+  'Clinical data' AS file_category,
+  file.file_type AS file_type,
+  file.file_description AS file_description,
+  file.file_size AS file_size,
+  file.md5sum AS md5sum,
+  st.study_id AS study_id,
+  st.phs_accession as phs_accession,
+  st.study_acronym as study_acronym,
+  st.study_short_title as study_short_title,
+  p.participant_id AS participant_id,
+  null AS sample_id,
+  null as combined_filters,
+  COLLECT(DISTINCT {
+      race: races,
+      sex_at_birth: p.sex_at_birth,
+      ethnicity: ethnicities
+  }) AS participant_filters,
+  COLLECT(DISTINCT {
+      age_at_diagnosis: dg.age_at_diagnosis,
+      diagnosis_anatomic_site: dg.anatomic_site,
+      disease_phase: dg.disease_phase,
+      diagnosis_classification_system: dg.diagnosis_classification_system,
+      diagnosis_verification_status: dg.diagnosis_verification_status,
+      diagnosis_basis: dg.diagnosis_basis,
+      diagnosis_comment: dg.diagnosis_comment,
+      diagnosis_classification: dg.diagnosis_classification
+  }) AS diagnosis_filters,
+  COLLECT(DISTINCT fu.vital_status) as vital_status,
+  COLLECT(DISTINCT {
+      sample_anatomic_site: sm.anatomic_site,
+      participant_age_at_collection: sm.participant_age_at_collection,
+      sample_tumor_status: sm.sample_tumor_status,
+      tumor_classification: sm.tumor_classification
+  }) AS sample_filters,
+  COLLECT(DISTINCT stf.grant_id) as grant_id,
+  COLLECT(DISTINCT stp.institution) as institution,      
+  null AS library_selection,
+  null AS library_source,
+  null AS library_strategy
+UNION ALL
+with st
+MATCH (file:methylation_array_file)
+MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_methylation_array_file]-(file)
+MATCH (st)&lt;-[:of_participant]-(p)
+OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
+OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
+UNWIND apoc.text.split(p.race, ';') AS races
+with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
+RETURN DISTINCT
+  file.id as id,
+  p.id as pid,
+  file.methylation_array_file_id AS file_id,
+  file.dcf_indexd_guid AS guid,
+  file.file_name AS file_name,
+  'Methylation array' AS file_category,
+  file.file_type AS file_type,
+  file.file_description AS file_description,
+  file.file_size AS file_size,
+  file.md5sum AS md5sum,
+  st.study_id AS study_id,
+  st.phs_accession as phs_accession,
+  st.study_acronym as study_acronym,
+  st.study_short_title as study_short_title,
+  p.participant_id AS participant_id,
+  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
+            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
+  null as combined_filters,
+  COLLECT(DISTINCT {
+      race: races,
+      sex_at_birth: p.sex_at_birth,
+      ethnicity: ethnicities
+  }) AS participant_filters,
+  COLLECT(DISTINCT {
+      age_at_diagnosis: dg.age_at_diagnosis,
+      diagnosis_anatomic_site: dg.anatomic_site,
+      disease_phase: dg.disease_phase,
+      diagnosis_classification_system: dg.diagnosis_classification_system,
+      diagnosis_verification_status: dg.diagnosis_verification_status,
+      diagnosis_basis: dg.diagnosis_basis,
+      diagnosis_comment: dg.diagnosis_comment,
+      diagnosis_classification: dg.diagnosis_classification
+  }) AS diagnosis_filters,
+  COLLECT(DISTINCT fu.vital_status) as vital_status,
+  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })
+            ELSE apoc.coll.union(COLLECT(DISTINCT {
+                              sample_anatomic_site: sm1.anatomic_site,
+                              participant_age_at_collection: sm1.participant_age_at_collection,
+                              sample_tumor_status: sm1.sample_tumor_status,
+                              tumor_classification: sm1.tumor_classification
+                          }), COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })) END AS sample_filters,
+  COLLECT(DISTINCT stf.grant_id) as grant_id,
+  COLLECT(DISTINCT stp.institution) as institution,
+  null AS library_selection,
+  null AS library_source,
+  null AS library_strategy
+UNION ALL
+with st
+MATCH (file:pathology_file)
+MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_pathology_file]-(file)
+MATCH (st)&lt;-[:of_participant]-(p)
+OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
+OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
+UNWIND apoc.text.split(p.race, ';') AS races
+with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
+RETURN DISTINCT
+  file.id as id,
+  p.id as pid,
+  file.pathology_file_id AS file_id,
+  file.dcf_indexd_guid AS guid,
+  file.file_name AS file_name,
+  'Pathology imaging' AS file_category,
+  file.file_type AS file_type,
+  file.file_description AS file_description,
+  file.file_size AS file_size,
+  file.md5sum AS md5sum,
+  st.study_id AS study_id,
+  st.phs_accession as phs_accession,
+  st.study_acronym as study_acronym,
+  st.study_short_title as study_short_title,
+  p.participant_id AS participant_id,
+  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
+            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
+  null as combined_filters,
+  COLLECT(DISTINCT {
+      race: races,
+      sex_at_birth: p.sex_at_birth,
+      ethnicity: ethnicities
+  }) AS participant_filters,
+  COLLECT(DISTINCT {
+      age_at_diagnosis: dg.age_at_diagnosis,
+      diagnosis_anatomic_site: dg.anatomic_site,
+      disease_phase: dg.disease_phase,
+      diagnosis_classification_system: dg.diagnosis_classification_system,
+      diagnosis_verification_status: dg.diagnosis_verification_status,
+      diagnosis_basis: dg.diagnosis_basis,
+      diagnosis_comment: dg.diagnosis_comment,
+      diagnosis_classification: dg.diagnosis_classification
+  }) AS diagnosis_filters,
+  COLLECT(DISTINCT fu.vital_status) as vital_status,
+  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })
+            ELSE apoc.coll.union(COLLECT(DISTINCT {
+                              sample_anatomic_site: sm1.anatomic_site,
+                              participant_age_at_collection: sm1.participant_age_at_collection,
+                              sample_tumor_status: sm1.sample_tumor_status,
+                              tumor_classification: sm1.tumor_classification
+                          }), COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })) END AS sample_filters,
+  COLLECT(DISTINCT stf.grant_id) as grant_id,
+  COLLECT(DISTINCT stp.institution) as institution,
+  file.library_selection AS library_selection,
+  file.library_source AS library_source,
+  file.library_strategy AS library_strategy
+UNION ALL
+with st
+MATCH (file:radiology_file)
+MATCH (p:participant)&lt;-[:of_radiology_file]-(file)
+MATCH (st)&lt;-[:of_participant]-(p)
+OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)
+OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
+OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
+UNWIND apoc.text.split(p.race, ';') AS races
+RETURN DISTINCT
+  file.id as id,
+  p.id as pid,
+  file.radiology_file_id AS file_id,
+  file.dcf_indexd_guid AS guid,
+  file.file_name AS file_name,
+  'Radiology imaging' AS file_category,
+  file.file_type AS file_type,
+  file.file_description AS file_description,
+  file.file_size AS file_size,
+  file.md5sum AS md5sum,
+  st.study_id AS study_id,
+  st.phs_accession as phs_accession,
+  st.study_acronym as study_acronym,
+  st.study_short_title as study_short_title,
+  p.participant_id AS participant_id,
+  null AS sample_id,
+  null as combined_filters,
+  COLLECT(DISTINCT {
+      race: races,
+      sex_at_birth: p.sex_at_birth,
+      ethnicity: ethnicities
+  }) AS participant_filters,
+  COLLECT(DISTINCT {
+      age_at_diagnosis: dg.age_at_diagnosis,
+      diagnosis_anatomic_site: dg.anatomic_site,
+      disease_phase: dg.disease_phase,
+      diagnosis_classification_system: dg.diagnosis_classification_system,
+      diagnosis_verification_status: dg.diagnosis_verification_status,
+      diagnosis_basis: dg.diagnosis_basis,
+      diagnosis_comment: dg.diagnosis_comment,
+      diagnosis_classification: dg.diagnosis_classification
+  }) AS diagnosis_filters,
+  COLLECT(DISTINCT fu.vital_status) as vital_status,
+  COLLECT(DISTINCT {
+      sample_anatomic_site: sm.anatomic_site,
+      participant_age_at_collection: sm.participant_age_at_collection,
+      sample_tumor_status: sm.sample_tumor_status,
+      tumor_classification: sm.tumor_classification
+  }) AS sample_filters,
+  COLLECT(DISTINCT stf.grant_id) as grant_id,
+  COLLECT(DISTINCT stp.institution) as institution,
+  null AS library_selection,
+  null AS library_source,
+  null AS library_strategy
+UNION ALL
+with st
+MATCH (file:single_cell_sequencing_file)
+MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_single_cell_sequencing_file]-(file)
+MATCH (st)&lt;-[:of_participant]-(p)
+OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
+OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
+UNWIND apoc.text.split(p.race, ';') AS races
+with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
+RETURN DISTINCT
+  file.id as id,
+  p.id as pid,
+  file.single_cell_sequencing_file_id AS file_id,
+  file.dcf_indexd_guid AS guid,
+  file.file_name AS file_name,
+  'Single Cell Sequencing' AS file_category,
+  file.file_type AS file_type,
+  file.file_description AS file_description,
+  file.file_size AS file_size,
+  file.md5sum AS md5sum,
+  st.study_id AS study_id,
+  st.phs_accession as phs_accession,
+  st.study_acronym as study_acronym,
+  st.study_short_title as study_short_title,
+  p.participant_id AS participant_id,
+  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
+            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
+  null as combined_filters,
+  COLLECT(DISTINCT {
+      race: races,
+      sex_at_birth: p.sex_at_birth,
+      ethnicity: ethnicities
+  }) AS participant_filters,
+  COLLECT(DISTINCT {
+      age_at_diagnosis: dg.age_at_diagnosis,
+      diagnosis_anatomic_site: dg.anatomic_site,
+      disease_phase: dg.disease_phase,
+      diagnosis_classification_system: dg.diagnosis_classification_system,
+      diagnosis_verification_status: dg.diagnosis_verification_status,
+      diagnosis_basis: dg.diagnosis_basis,
+      diagnosis_comment: dg.diagnosis_comment,
+      diagnosis_classification: dg.diagnosis_classification
+  }) AS diagnosis_filters,
+  COLLECT(DISTINCT fu.vital_status) as vital_status,
+  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })
+            ELSE apoc.coll.union(COLLECT(DISTINCT {
+                              sample_anatomic_site: sm1.anatomic_site,
+                              participant_age_at_collection: sm1.participant_age_at_collection,
+                              sample_tumor_status: sm1.sample_tumor_status,
+                              tumor_classification: sm1.tumor_classification
+                          }), COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })) END AS sample_filters,
+  COLLECT(DISTINCT stf.grant_id) as grant_id,
+  COLLECT(DISTINCT stp.institution) as institution,
+  file.library_selection AS library_selection,
+  file.library_source AS library_source,
+  file.library_strategy AS library_strategy
+UNION ALL
+with st
+MATCH (file:sequencing_file)
+MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_sequencing_file]-(file)
+MATCH (st)&lt;-[:of_participant]-(p)
+OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
+OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
+UNWIND apoc.text.split(p.race, ';') AS races
+with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
+RETURN DISTINCT
+  file.id as id,
+  p.id as pid,
+  file.sequencing_file_id AS file_id,
+  file.dcf_indexd_guid AS guid,
+  file.file_name AS file_name,
+  'Sequencing' AS file_category,
+  file.file_type AS file_type,
+  file.file_description AS file_description,
+  file.file_size AS file_size,
+  file.md5sum AS md5sum,
+  st.study_id AS study_id,
+  st.phs_accession as phs_accession,
+  st.study_acronym as study_acronym,
+  st.study_short_title as study_short_title,
+  p.participant_id AS participant_id,
+  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
+            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
+  null as combined_filters,
+  COLLECT(DISTINCT {
+      race: races,
+      sex_at_birth: p.sex_at_birth,
+      ethnicity: ethnicities
+  }) AS participant_filters,
+  COLLECT(DISTINCT {
+      age_at_diagnosis: dg.age_at_diagnosis,
+      diagnosis_anatomic_site: dg.anatomic_site,
+      disease_phase: dg.disease_phase,
+      diagnosis_classification_system: dg.diagnosis_classification_system,
+      diagnosis_verification_status: dg.diagnosis_verification_status,
+      diagnosis_basis: dg.diagnosis_basis,
+      diagnosis_comment: dg.diagnosis_comment,
+      diagnosis_classification: dg.diagnosis_classification
+  }) AS diagnosis_filters,
+  COLLECT(DISTINCT fu.vital_status) as vital_status,
+  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })
+            ELSE apoc.coll.union(COLLECT(DISTINCT {
+                              sample_anatomic_site: sm1.anatomic_site,
+                              participant_age_at_collection: sm1.participant_age_at_collection,
+                              sample_tumor_status: sm1.sample_tumor_status,
+                              tumor_classification: sm1.tumor_classification
+                          }), COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })) END AS sample_filters,
+  COLLECT(DISTINCT stf.grant_id) as grant_id,
+  COLLECT(DISTINCT stp.institution) as institution,
+  file.library_selection AS library_selection,
+  file.library_source AS library_source,
+  file.library_strategy AS library_strategy
+UNION ALL
+with st
+MATCH (file:cytogenomic_file)
+MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_cytogenomic_file]-(file)
+MATCH (st)&lt;-[:of_participant]-(p)
+OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
+OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+UNWIND apoc.text.split(p.ethnicity, ';') AS ethnicities
+UNWIND apoc.text.split(p.race, ';') AS races
+with file, p, sm1, sm, st, ethnicities, races, fu, dg, stf, stp
+RETURN DISTINCT
+  file.id as id,
+  p.id as pid,
+  file.cytogenomic_file_id AS file_id,
+  file.dcf_indexd_guid AS guid,
+  file.file_name AS file_name,
+  'Cytogenomic' AS file_category,
+  file.file_type AS file_type,
+  file.file_description AS file_description,
+  file.file_size AS file_size,
+  file.md5sum AS md5sum,
+  st.study_id AS study_id,
+  st.phs_accession as phs_accession,
+  st.study_acronym as study_acronym,
+  st.study_short_title as study_short_title,
+  p.participant_id AS participant_id,
+  CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
+            ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
+  null as combined_filters,
+  COLLECT(DISTINCT {
+      race: races,
+      sex_at_birth: p.sex_at_birth,
+      ethnicity: ethnicities
+  }) AS participant_filters,
+  COLLECT(DISTINCT {
+      age_at_diagnosis: dg.age_at_diagnosis,
+      diagnosis_anatomic_site: dg.anatomic_site,
+      disease_phase: dg.disease_phase,
+      diagnosis_classification_system: dg.diagnosis_classification_system,
+      diagnosis_verification_status: dg.diagnosis_verification_status,
+      diagnosis_basis: dg.diagnosis_basis,
+      diagnosis_comment: dg.diagnosis_comment,
+      diagnosis_classification: dg.diagnosis_classification
+  }) AS diagnosis_filters,
+  COLLECT(DISTINCT fu.vital_status) as vital_status,
+  CASE sm1.sample_id WHEN sm.sample_id THEN COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })
+            ELSE apoc.coll.union(COLLECT(DISTINCT {
+                              sample_anatomic_site: sm1.anatomic_site,
+                              participant_age_at_collection: sm1.participant_age_at_collection,
+                              sample_tumor_status: sm1.sample_tumor_status,
+                              tumor_classification: sm1.tumor_classification
+                          }), COLLECT(DISTINCT {
+                              sample_anatomic_site: sm.anatomic_site,
+                              participant_age_at_collection: sm.participant_age_at_collection,
+                              sample_tumor_status: sm.sample_tumor_status,
+                              tumor_classification: sm.tumor_classification
+                          })) END AS sample_filters,
+  COLLECT(DISTINCT stf.grant_id) as grant_id,
+  COLLECT(DISTINCT stp.institution) as institution,
+  null AS library_selection,
+  null AS library_source,
+  null AS library_strategy
+UNION ALL
+with st
+MATCH (file)
+WHERE (file:sequencing_file OR file:pathology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
+MATCH (st)&lt;-[:of_cell_line|of_pdx]-(cl)&lt;--(sm:sample)
+Where (cl: cell_line or cl: pdx)
+MATCH (sm)&lt;--(file)
+OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+OPTIONAL MATCH (st)&lt;--(p:participant)&lt;-[:of_diagnosis]-(dg:diagnosis)
+OPTIONAL MATCH (st)&lt;--(p)&lt;-[:of_follow_up]-(fu:follow_up)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+with file, sm, st, fu, dg, stf, stp
+RETURN DISTINCT
+  file.id as id,
+  null as pid,
+  CASE LABELS(file)[0]
+        WHEN 'sequencing_file' THEN file.sequencing_file_id
+        WHEN 'single_cell_sequencing_file' THEN file.single_cell_sequencing_file_id
+        WHEN 'cytogenomic_file' THEN file.cytogenomic_file_id
+        WHEN 'pathology_file' THEN file.pathology_file_id
+        WHEN 'methylation_array_file' THEN file.methylation_array_file_id END AS file_id,
+  file.dcf_indexd_guid AS guid,
+  file.file_name AS file_name,
+  CASE LABELS(file)[0]
+        WHEN 'sequencing_file' THEN 'Sequencing'
+        WHEN 'single_cell_sequencing_file' THEN 'Single Cell Sequencing'
+        WHEN 'cytogenomic_file' THEN 'Cytogenomic'
+        WHEN 'pathology_file' THEN 'Pathology imaging'
+        WHEN 'methylation_array_file' THEN 'Methylation array' END AS file_category,
+  file.file_type AS file_type,
+  file.file_description AS file_description,
+  file.file_size AS file_size,
+  file.md5sum AS md5sum,
+  st.study_id AS study_id,
+  st.phs_accession as phs_accession,
+  st.study_acronym as study_acronym,
+  st.study_short_title as study_short_title,
+  null AS participant_id,
+  sm.sample_id AS sample_id,
+  null as combined_filters,
+  null AS participant_filters,
+  COLLECT(DISTINCT {
+      age_at_diagnosis: dg.age_at_diagnosis,
+      diagnosis_anatomic_site: dg.anatomic_site,
+      disease_phase: dg.disease_phase,
+      diagnosis_classification_system: dg.diagnosis_classification_system,
+      diagnosis_verification_status: dg.diagnosis_verification_status,
+      diagnosis_basis: dg.diagnosis_basis,
+      diagnosis_comment: dg.diagnosis_comment,
+      diagnosis_classification: dg.diagnosis_classification
+  }) AS diagnosis_filters,
+  COLLECT(DISTINCT fu.vital_status) as vital_status,
+  COLLECT(DISTINCT {
+      sample_anatomic_site: sm.anatomic_site,
+      participant_age_at_collection: sm.participant_age_at_collection,
+      sample_tumor_status: sm.sample_tumor_status,
+      tumor_classification: sm.tumor_classification
+  }) AS sample_filters,
+  COLLECT(DISTINCT stf.grant_id) as grant_id,
+  COLLECT(DISTINCT stp.institution) as institution,
+  CASE LABELS(file)[0]
+            WHEN 'sequencing_file' THEN file.library_selection
+            WHEN 'single_cell_sequencing_file' THEN file.library_selection
+            ELSE null END AS library_selection,
+  CASE LABELS(file)[0]
+            WHEN 'sequencing_file' THEN file.library_source
+            WHEN 'single_cell_sequencing_file' THEN file.library_source
+            ELSE null END AS library_source,
+  CASE LABELS(file)[0]
+            WHEN 'sequencing_file' THEN file.library_strategy
+            WHEN 'single_cell_sequencing_file' THEN file.library_strategy
+            ELSE null END AS library_strategy
+}
+with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, pid, participant_id, sample_id, participant_filters,diagnosis_filters, vital_status, sample_filters, grant_id, institution,library_selection,library_source,library_strategy
+unwind participant_filters as participant_filter
+with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, pid, participant_id, sample_id, participant_filter,diagnosis_filters, vital_status, sample_filters, grant_id, institution,library_selection,library_source,library_strategy
+where  participant_filter.sex_at_birth in ['Male'] and ANY(element IN ['Unknown'] WHERE element IN participant_filter.race)  
+unwind diagnosis_filters as diagnosis_filter
+with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, pid, participant_id, sample_id,diagnosis_filter, vital_status, sample_filters, grant_id, institution,library_selection,library_source,library_strategy
+ with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, pid, participant_id, sample_id, vital_status, sample_filters, grant_id, institution,library_selection,library_source,library_strategy
+ unwind sample_filters as sample_filter
+with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, pid, participant_id, sample_id, sample_filter, grant_id, institution,library_selection,library_source,library_strategy
+ with distinct id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, pid, participant_id, sample_id, grant_id, institution,library_selection,library_source,library_strategy
+call {
+  with id, guid, file_name, file_category, file_type, file_description, file_size, md5sum, study_id, phs_accession, study_acronym, study_short_title, pid, participant_id, sample_id, grant_id, institution,library_selection,library_source,library_strategy
+  return id as fid, guid as dig, file_name as fn, file_category as fc, file_type as ft, file_description as fd, file_size as fsize, md5sum as md5, study_id as sid, phs_accession as pa, study_acronym as sa, study_short_title as sst, pid as u_p_id, participant_id as p_id, sample_id as smid, grant_id as gid, institution as istt,library_selection as ls,library_source as lis,library_strategy as listr
+  UNION ALL
+  with study_id
+  MATCH (file:clinical_measure_file)
+  MATCH (stu:study)&lt;-[:of_clinical_measure_file]-(file)
+  where stu.study_id = study_id
+  OPTIONAL MATCH (stu)&lt;-[:of_study_personnel]-(stp:study_personnel)
+  OPTIONAL MATCH (stu)&lt;-[:of_study_funding]-(stf:study_funding)
+  With file, stu, stf, stp
+  RETURN DISTINCT
+    file.id as fid,
+    file.dcf_indexd_guid AS dig,
+    file.file_name AS fn,
+    'Clinical data' AS fc,
+    file.file_type AS ft,
+    file.file_description AS fd,
+    file.file_size AS fsize,
+    file.md5sum AS md5,
+    stu.study_id AS sid,
+    stu.phs_accession as pa,
+    stu.study_acronym as sa,
+    stu.study_short_title as sst,
+    null AS p_id,
+    null AS u_p_id,
+    null AS smid,
+    COLLECT(DISTINCT stf.grant_id) as gid,
+    COLLECT(DISTINCT stp.institution) as istt,
+    null AS ls,
+    null AS lis,
+    null AS listr
+}
+with fid as id, dig as guid, fn as file_name, fc as file_category, ft as file_type, fd as file_description, fsize as file_size, md5 as md5sum, sid as study_id, pa as phs_accession, sa as study_acronym, sst as study_short_title, u_p_id as unique_participant_id, p_id as participant_id, smid as sample_id, gid as grant_id, istt as institution,ls as library_selection,lis as library_source,listr as library_strategy
+ with DISTINCT id, study_id, unique_participant_id, sample_id
+with id, study_id, unique_participant_id, case sample_id when null then [null] else apoc.text.split(sample_id, ',') end as sample_ids
+unwind sample_ids as single_sample_id
+return count(distinct study_id) as Studies, count(distinct unique_participant_id) as Participants, count(distinct single_sample_id) as Samples, count(distinct id) as Files</t>
+  </si>
+  <si>
+    <t>MATCH (p:participant)--&gt;(st:study)
+where st.phs_accession in ['phs002620']
+optional MATCH (p)&lt;-[:of_sample]-(sm1:sample)&lt;--(cl)&lt;--(sm2:sample)
+WHERE (cl: cell_line or cl: pdx)
+optional Match (sm2)&lt;--(file)
+WHERE (file: sequencing_file OR file:pathology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file) 
+with p, case COLLECT(distinct sm1) when [] then []
+                else COLLECT(DISTINCT {
+                        sample_anatomic_site: sm1.anatomic_site,
+                        participant_age_at_collection: sm1.participant_age_at_collection,
+                        sample_tumor_status: sm1.sample_tumor_status,
+                        tumor_classification: sm1.tumor_classification,
+                        assay_method: CASE LABELS(file)[0]
+                                  WHEN 'sequencing_file' THEN 'Sequencing'
+                                  WHEN 'single_cell_sequencing_file' THEN 'Single Cell Sequencing'
+                                  WHEN 'cytogenomic_file' THEN 'Cytogenomic'
+                                  WHEN 'pathology_file' THEN 'Pathology imaging'
+                                  WHEN 'methylation_array_file' THEN 'Methylation array'
+                                  ELSE null END,
+                        file_type: CASE LABELS(file)[0]
+                                  When null then null
+                                  else file.file_type end,
+                        library_selection: CASE LABELS(file)[0]
+                                      WHEN 'sequencing_file' THEN file.library_selection
+                                      WHEN 'single_cell_sequencing_file' THEN file.library_selection
+                                      ELSE null END,
+                        library_source: CASE LABELS(file)[0]
+                                      WHEN 'sequencing_file' THEN file.library_source
+                                      WHEN 'single_cell_sequencing_file' THEN file.library_source
+                                      ELSE null END,
+                        library_strategy: CASE LABELS(file)[0]
+                                      WHEN 'sequencing_file' THEN file.library_strategy
+                                      WHEN 'single_cell_sequencing_file' THEN file.library_strategy
+                                      ELSE null END
+                    }) end AS sample1,
+                    case COLLECT(distinct sm2) 
+                    when [] then []
+                    else COLLECT(DISTINCT {
+                        sample_anatomic_site: sm2.anatomic_site,
+                        participant_age_at_collection: sm2.participant_age_at_collection,
+                        sample_tumor_status: sm2.sample_tumor_status,
+                        tumor_classification: sm2.tumor_classification,
+                        assay_method: CASE LABELS(file)[0]
+                                  WHEN 'sequencing_file' THEN 'Sequencing'
+                                  WHEN 'single_cell_sequencing_file' THEN 'Single Cell Sequencing'
+                                  WHEN 'cytogenomic_file' THEN 'Cytogenomic'
+                                  WHEN 'pathology_file' THEN 'Pathology imaging'
+                                  WHEN 'methylation_array_file' THEN 'Methylation array'
+                                  ELSE null END,
+                        file_type: CASE LABELS(file)[0]
+                                  When null then null
+                                  else file.file_type end,
+                        library_selection: CASE LABELS(file)[0]
+                                      WHEN 'sequencing_file' THEN file.library_selection
+                                      WHEN 'single_cell_sequencing_file' THEN file.library_selection
+                                      ELSE null END,
+                        library_source: CASE LABELS(file)[0]
+                                      WHEN 'sequencing_file' THEN file.library_source
+                                      WHEN 'single_cell_sequencing_file' THEN file.library_source
+                                      ELSE null END,
+                        library_strategy: CASE LABELS(file)[0]
+                                      WHEN 'sequencing_file' THEN file.library_strategy
+                                      WHEN 'single_cell_sequencing_file' THEN file.library_strategy
+                                      ELSE null END
+                    }) end AS sample2
+with p, apoc.coll.union(sample1,sample2) as cell_line_pdx_file_filters
+OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)&lt;--(file)
+WHERE (file: sequencing_file OR file:pathology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
+with p, cell_line_pdx_file_filters, COLLECT(DISTINCT {
+              sample_anatomic_site: sm.anatomic_site,
+              participant_age_at_collection: sm.participant_age_at_collection,
+              sample_tumor_status: sm.sample_tumor_status,
+              tumor_classification: sm.tumor_classification,
+              assay_method: CASE LABELS(file)[0]
+                        WHEN 'sequencing_file' THEN 'Sequencing'
+                        WHEN 'single_cell_sequencing_file' THEN 'Single Cell Sequencing'
+                        WHEN 'cytogenomic_file' THEN 'Cytogenomic'
+                        WHEN 'pathology_file' THEN 'Pathology imaging'
+                        WHEN 'methylation_array_file' THEN 'Methylation array' END,
+              file_type: file.file_type,
+              library_selection: CASE LABELS(file)[0]
+                            WHEN 'sequencing_file' THEN file.library_selection
+                            WHEN 'single_cell_sequencing_file' THEN file.library_selection
+                            ELSE null END,
+              library_source: CASE LABELS(file)[0]
+                            WHEN 'sequencing_file' THEN file.library_source
+                              WHEN 'single_cell_sequencing_file' THEN file.library_source
+                            ELSE null END,
+              library_strategy: CASE LABELS(file)[0]
+                            WHEN 'sequencing_file' THEN file.library_strategy
+                            WHEN 'single_cell_sequencing_file' THEN file.library_strategy
+                            ELSE null END
+          }) AS general_file_filters
+OPTIONAL Match (p)&lt;-[:of_sample]-(sm:sample)
+OPTIONAL MATCH (p)&lt;-[:of_clinical_measure_file]-(file1:clinical_measure_file)
+with p, cell_line_pdx_file_filters, general_file_filters,sm, COLLECT(DISTINCT file1.file_type) as file1_types
+UNWIND (case file1_types when [] then [null] else file1_types end)  AS types_1
+with p, cell_line_pdx_file_filters, general_file_filters, COLLECT(DISTINCT {
+          sample_anatomic_site: sm.anatomic_site,
+          participant_age_at_collection: sm.participant_age_at_collection,
+          sample_tumor_status: sm.sample_tumor_status,
+          tumor_classification: sm.tumor_classification,
+          assay_method: CASE types_1 when null then null else 'Clinical data' end,
+          file_type: types_1,
+          library_selection: null,
+          library_source: null,
+          library_strategy: null
+  }) as participant_clinical_measure_file_filters
+OPTIONAL Match (p)&lt;-[:of_sample]-(sm:sample)
+OPTIONAL MATCH (p)&lt;-[:of_radiology_file]-(file1:radiology_file)
+with p, cell_line_pdx_file_filters, general_file_filters, participant_clinical_measure_file_filters, sm, COLLECT(DISTINCT file1.file_type) as file1_types
+UNWIND (case file1_types when [] then [null] else file1_types end)  AS types_1
+with p, cell_line_pdx_file_filters, general_file_filters, participant_clinical_measure_file_filters, COLLECT(DISTINCT {
+          sample_anatomic_site: sm.anatomic_site,
+          participant_age_at_collection: sm.participant_age_at_collection,
+          sample_tumor_status: sm.sample_tumor_status,
+          tumor_classification: sm.tumor_classification,
+          assay_method: CASE types_1 when null then null else 'Radiology imaging' end,
+          file_type: types_1,
+          library_selection: null,
+          library_source: null,
+          library_strategy: null
+  }) as participant_radiology_file_filters
+OPTIONAL MATCH (p)&lt;-[*..4]-(file)
+WHERE (file:clinical_measure_file OR file: sequencing_file OR file:pathology_file OR file:radiology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
+OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
+OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
+OPTIONAL MATCH (st:study)&lt;-[:of_participant]-(p)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+WITH p, cell_line_pdx_file_filters, general_file_filters, participant_clinical_measure_file_filters, participant_radiology_file_filters, file, fu, st, stf, stp, dg
+with DISTINCT
+  p.id as id,
+  p.participant_id as participant_id,
+  apoc.text.split(p.race, ';') as race,
+  p.race as race_str,
+  p.sex_at_birth as sex_at_birth,
+  p.ethnicity as ethnicity_str,
+  apoc.text.split(p.ethnicity, ';') as ethnicity,
+  p.alternate_participant_id as alternate_participant_id,
+  COLLECT(DISTINCT {
+      age_at_diagnosis: dg.age_at_diagnosis,
+      diagnosis_anatomic_site: dg.anatomic_site,
+      disease_phase: dg.disease_phase,
+      diagnosis_classification_system: dg.diagnosis_classification_system,
+      diagnosis_verification_status: dg.diagnosis_verification_status,
+      diagnosis_basis: dg.diagnosis_basis,
+      diagnosis_comment: dg.diagnosis_comment,
+      diagnosis_classification: dg.diagnosis_classification
+  }) AS diagnosis_filters,
+  COLLECT(DISTINCT fu.vital_status) as vital_status,
+  apoc.coll.union(cell_line_pdx_file_filters, general_file_filters) + participant_clinical_measure_file_filters + participant_radiology_file_filters AS sample_file_filters,
+  st.study_id as study_id,
+  st.phs_accession as phs_accession,
+  COLLECT(DISTINCT stf.grant_id) as grant_id,
+  COLLECT(DISTINCT stp.institution) as institution,
+  st.study_acronym as study_acronym,
+  st.study_short_title as study_short_title
+    with id, participant_id, phs_accession, sex_at_birth, race_str, ethnicity_str, race, ethnicity, alternate_participant_id, diagnosis_filters, vital_status, sample_file_filters
+  where   sex_at_birth in ['Male'] and ANY(element IN ['Unknown'] WHERE element IN race)  
+  unwind diagnosis_filters as diagnosis_filter
+  with id, participant_id, phs_accession, sex_at_birth, race_str, ethnicity_str, alternate_participant_id, diagnosis_filter, vital_status, sample_file_filters
+    with id, participant_id, phs_accession, sex_at_birth, race_str, ethnicity_str, alternate_participant_id, vital_status, sample_file_filters
+  unwind sample_file_filters as sample_file_filter
+  with id, participant_id, phs_accession, sex_at_birth, race_str, ethnicity_str, alternate_participant_id, sample_file_filter
+   with distinct id, participant_id, phs_accession, sex_at_birth, race_str, ethnicity_str, alternate_participant_id
+  return
+  coalesce(participant_id, '') AS `Participant ID`,
+  coalesce(phs_accession, '') AS `Study ID`,
+  coalesce(sex_at_birth, '') AS `Sex` ,
+  coalesce(race_str, '') AS `Race`,
+  coalesce(ethnicity_str, '') AS `Ethnicity` ,
+  coalesce(alternate_participant_id, '') AS `Alternate ID`
+  Order by participant_id Limit 100</t>
   </si>
 </sst>
 </file>
@@ -2399,8 +2226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2434,10 +2261,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -2451,10 +2278,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -2468,10 +2295,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -2485,10 +2312,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -2502,10 +2329,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>

</xml_diff>